<commit_message>
fixed rotated rectangle to AABB transformation
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Atlas\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Atlas\src\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Размечено</t>
   </si>
@@ -78,31 +78,16 @@
     <t>2 - Классификация кода производителя</t>
   </si>
   <si>
-    <t>resize 320x320, нормализация</t>
-  </si>
-  <si>
-    <t>Реформатирование в ч/б + параметры теста 1</t>
-  </si>
-  <si>
     <t>Версия модели 1</t>
   </si>
   <si>
     <t>Версия модели 2</t>
   </si>
   <si>
-    <t>Параметры теста 1</t>
-  </si>
-  <si>
     <t>Параметры предобработки изображений</t>
   </si>
   <si>
     <t>Изменения в модели</t>
-  </si>
-  <si>
-    <t>Базовая модель: MobileNetV2</t>
-  </si>
-  <si>
-    <t>Линейная активация, Dropout(0,3)</t>
   </si>
 </sst>
 </file>
@@ -491,7 +476,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,16 +506,16 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
@@ -540,27 +525,7 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="E2">
-        <v>5.4100000000000002E-2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="L2" t="s">
         <v>15</v>
       </c>
@@ -569,24 +534,7 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E3">
-        <v>0.1459</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="I3" s="6"/>
       <c r="L3" t="s">
         <v>16</v>
       </c>
@@ -595,27 +543,7 @@
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>1.24E-2</v>
-      </c>
-      <c r="E4">
-        <v>8.7099999999999997E-2</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -747,12 +675,14 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
+      <c r="E26" s="7"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
+      <c r="E27" s="7"/>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -774,24 +704,30 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="4"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
model modifications, updated meta
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Размечено</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Неудовлетворительные, модель сложновата и для корректной работы нужно значительное время, чтобы разобраться</t>
+  </si>
+  <si>
+    <t>Эксперименты с Resnet18</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.4, Val IoU: 0.32. Первые относительно рабочие результаты. Точность всё ещё крайне низкая, но можно дорабатывать отсюда.</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -208,7 +214,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -492,7 +506,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +515,7 @@
     <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -553,14 +567,14 @@
       <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>22</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -579,201 +593,217 @@
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
@@ -785,7 +815,7 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>

</xml_diff>

<commit_message>
small meta update. Final version 4
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Размечено</t>
   </si>
@@ -109,6 +109,36 @@
   </si>
   <si>
     <t>Train IoU: 0.4, Val IoU: 0.32. Первые относительно рабочие результаты. Точность всё ещё крайне низкая, но можно дорабатывать отсюда.</t>
+  </si>
+  <si>
+    <t>Небольшая аугментация датасета</t>
+  </si>
+  <si>
+    <t>ID коммита на git</t>
+  </si>
+  <si>
+    <t>a2c6d00</t>
+  </si>
+  <si>
+    <t>76721e3</t>
+  </si>
+  <si>
+    <t>параметры теста 4</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.29, Val IoU: 0.34. Незначительные улучшения, возможно нужно больше эпох.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.36, Val IoU: 0.39. Многообещающие улучшения, модель достаточно часто попадает в номер, но либо слегка широко, либо со сдвигом.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.39, Val IoU: 0.44 </t>
+  </si>
+  <si>
+    <t>Train IoU: 0.39, Val IoU: 0.44. Для этой версии достигнут пик обучения.</t>
+  </si>
+  <si>
+    <t>параметры теста 1, случайные аугментации внутри объекта датасета (переворот, смена масштаба)</t>
   </si>
 </sst>
 </file>
@@ -142,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -201,11 +231,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -214,15 +268,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -503,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,12 +584,14 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -538,17 +610,21 @@
       <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -564,17 +640,19 @@
       <c r="F2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="7"/>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -590,17 +668,19 @@
       <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="7"/>
+      <c r="K3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -616,196 +696,309 @@
       <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G9" s="8"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="8"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="8"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G12" s="8"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="8"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="8"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="8"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="8"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="8"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="8"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="8"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="8"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="8"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="8"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="8"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G26" s="8"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="8"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="8"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="9"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G29" s="8"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="9"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="8"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -814,40 +1007,42 @@
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="9"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="G32" s="12"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="7"/>
+      <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="G34" s="7"/>
+      <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="G36" s="7"/>
+      <c r="G36" s="12"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="G38" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
loss function changed to IoU
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -117,9 +117,6 @@
     <t>ID коммита на git</t>
   </si>
   <si>
-    <t>a2c6d00</t>
-  </si>
-  <si>
     <t>76721e3</t>
   </si>
   <si>
@@ -139,6 +136,10 @@
   </si>
   <si>
     <t>параметры теста 1, случайные аугментации внутри объекта датасета (переворот, смена масштаба)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a96e277
+</t>
   </si>
 </sst>
 </file>
@@ -259,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -293,6 +294,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -576,7 +580,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +707,7 @@
         <v>27</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="7"/>
     </row>
@@ -724,13 +728,13 @@
         <v>28</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="J5" s="7"/>
     </row>
@@ -748,10 +752,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="17"/>
       <c r="J6" s="7"/>
@@ -770,10 +774,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="7"/>
@@ -792,10 +796,10 @@
         <v>4</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="17"/>
       <c r="J8" s="7"/>

</xml_diff>

<commit_message>
loss function changed to 0.7xMSE+0.3xIoU
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Размечено</t>
   </si>
@@ -140,6 +140,15 @@
   <si>
     <t xml:space="preserve">a96e277
 </t>
+  </si>
+  <si>
+    <t>Заменена функция потерь на основанную на IoU.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.3, Val IoU: 0.3. Результаты хуже предыдущей версии. Возможно нужно больше эпох, либо корректировка метрики.</t>
+  </si>
+  <si>
+    <t>f01c369</t>
   </si>
 </sst>
 </file>
@@ -260,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -295,6 +304,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,14 +592,14 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -611,7 +623,7 @@
       <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="10" t="s">
@@ -641,7 +653,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -669,7 +681,7 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -697,7 +709,7 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -724,7 +736,7 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="8" t="s">
@@ -804,13 +816,31 @@
       <c r="I8" s="17"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="17"/>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>40</v>
+      </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1010,7 +1040,7 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="8"/>
       <c r="H31" s="15"/>
       <c r="I31" s="17"/>
@@ -1022,7 +1052,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="12"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
image rotation in preprocessing test
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Размечено</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Train IoU: 0.45, Val IoU: 0.41. Теоретически такая модель может быть дообучена до результатов чуть выше версии 6 (IoU~0.55), но её обучение занимает почти в 10 раз больше времени. Пока что откажусь от этой идеи.</t>
+  </si>
+  <si>
+    <t>Идеи улучшения: попробовать реализовать все повороты изображения, как-то внедрить IoU в метрику, но учесть, что очень важно минимальное расстояние между центрами (возможно, добавить только его)</t>
   </si>
 </sst>
 </file>
@@ -291,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -306,29 +309,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -611,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,45 +635,46 @@
     <col min="6" max="6" width="32.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="61.28515625" style="9" customWidth="1"/>
     <col min="12" max="12" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -678,19 +690,22 @@
       <c r="F2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="17"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="7"/>
-      <c r="K2" t="s">
+      <c r="K2" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="L2" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -709,16 +724,16 @@
       <c r="G3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="17"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="7"/>
-      <c r="K3" t="s">
+      <c r="K3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -737,15 +752,15 @@
       <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="13" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -764,15 +779,15 @@
       <c r="G5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="15" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -788,13 +803,13 @@
       <c r="G6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="17"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -810,13 +825,13 @@
       <c r="G7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -832,13 +847,13 @@
       <c r="G8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="17"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -857,15 +872,15 @@
       <c r="G9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -884,15 +899,15 @@
       <c r="G10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="13" t="s">
         <v>41</v>
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -908,13 +923,13 @@
       <c r="G11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="17"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -933,48 +948,49 @@
       <c r="G12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="15" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="17"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="17"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="17"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="17"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,8 +998,8 @@
         <v>16</v>
       </c>
       <c r="G17" s="8"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="17"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -991,8 +1007,8 @@
         <v>17</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="17"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1000,8 +1016,8 @@
         <v>18</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="17"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1009,8 +1025,8 @@
         <v>19</v>
       </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="17"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1018,8 +1034,8 @@
         <v>20</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="17"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,8 +1043,8 @@
         <v>21</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="17"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1036,8 +1052,8 @@
         <v>22</v>
       </c>
       <c r="G23" s="8"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="17"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1045,8 +1061,8 @@
         <v>23</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="17"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1054,8 +1070,8 @@
         <v>24</v>
       </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="17"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1063,8 +1079,8 @@
         <v>25</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="17"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1072,8 +1088,8 @@
         <v>26</v>
       </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="17"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1081,8 +1097,8 @@
         <v>27</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="17"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1090,8 +1106,8 @@
         <v>28</v>
       </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="17"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1099,8 +1115,8 @@
         <v>29</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="17"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1111,10 +1127,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="12"/>
+      <c r="F31" s="11"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="17"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1123,31 +1139,31 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="12"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
-      <c r="G34" s="12"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="11"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="11"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="11"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revert to v4, small visualization change
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Размечено</t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>Идеи улучшения: попробовать реализовать все повороты изображения, как-то внедрить IoU в метрику, но учесть, что очень важно минимальное расстояние между центрами (возможно, добавить только его)</t>
+  </si>
+  <si>
+    <t>параметры теста 4, к аугментациям добавляется поворот изображения на 90, 180 или 270 градусов</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.32, Val IoU: 0.37. Нужно проверить на большем количестве эпох.</t>
+  </si>
+  <si>
+    <t>8702ea4</t>
+  </si>
+  <si>
+    <t>параметры теста 12</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.30, Val IoU: 0.36. Аугментация не привела к улучшению точности.</t>
   </si>
 </sst>
 </file>
@@ -625,7 +640,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +720,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -957,21 +972,52 @@
       <c r="J12" s="7"/>
       <c r="K12" s="16"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="12"/>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I14" s="13"/>
       <c r="J14" s="7"/>
     </row>

</xml_diff>

<commit_message>
smaller changes to spatial attention
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -218,7 +218,7 @@
     <t>Модернизированное пространственное внимание, размер батча изменён обратно до 32</t>
   </si>
   <si>
-    <t>Train IoU: 0.50, Val IoU: 0.39. Изменение размера батча и нормалзация пока что мало влияют на точность.</t>
+    <t>Train IoU: 0.50, Val IoU: 0.39. Изменение размера батча и нормалзация пока что мало влияют на точность. Валидационный IoU в таком случае упирается в 0.4</t>
   </si>
 </sst>
 </file>
@@ -670,7 +670,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
loss function changed to MSE + center distance
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>Размечено</t>
   </si>
@@ -237,7 +237,22 @@
 </t>
   </si>
   <si>
-    <t>Изменение функции потерь на комбинацию MSE и IoU</t>
+    <t>1d4cdba</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.53, Val IoU: 0.51. Нужно поэкспериментировать с параметрами.</t>
+  </si>
+  <si>
+    <t>Изменение функции потерь на комбинацию MSE и IoU, в пропорции 70 на 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.47, Val IoU: 0.46. </t>
+  </si>
+  <si>
+    <t>MSE/IoU = 20/80</t>
+  </si>
+  <si>
+    <t>MSE/IoU = 10/90</t>
   </si>
 </sst>
 </file>
@@ -688,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1200,7 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1199,21 +1214,41 @@
         <v>13</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="12"/>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7"/>
     </row>
@@ -1221,7 +1256,21 @@
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="12"/>
       <c r="I21" s="13"/>
       <c r="J21" s="7"/>

</xml_diff>

<commit_message>
base model changed to efficientnet b4, batch size reduced to 16
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>Размечено</t>
   </si>
@@ -253,6 +253,21 @@
   </si>
   <si>
     <t>MSE/IoU = 10/90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.46, Val IoU: 0.46. </t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на комбинацию MSE и расстояния между центрами (50/50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.54, Val IoU: 0.54. </t>
+  </si>
+  <si>
+    <t>MSE/distance = 30/70</t>
+  </si>
+  <si>
+    <t>4df1807</t>
   </si>
 </sst>
 </file>
@@ -703,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,24 +1286,58 @@
       <c r="G21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="I21" s="13"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="13"/>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="12"/>
       <c r="I23" s="13"/>
       <c r="J23" s="7"/>

</xml_diff>

<commit_message>
changed image resize, batch size and changed loss function to MSE + IoU
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
   <si>
     <t>Размечено</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>4df1807</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.51, Val IoU: 0.47. Пока что результаты от замен функции потерь незначительные. В дальнейшем нужно доработать их и собрать все влияющие факторы в одну.</t>
+  </si>
+  <si>
+    <t>Замена базовой модели на EfficientNet B4, размер батча уменьшен до 16 для оптимальной скорости обучения новой модели</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.51, Val IoU: 0.50. Результат предыдущей лучшей версии достигается на меньшем количестве эпох и размере батча, но обучение длится в разы дольше.</t>
   </si>
 </sst>
 </file>
@@ -719,7 +728,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1328,7 @@
       </c>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -1338,16 +1347,34 @@
       <c r="G23" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="I23" s="13"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="12"/>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="I24" s="13"/>
       <c r="J24" s="7"/>
     </row>

</xml_diff>

<commit_message>
revert to version 12, small code cleanup
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Размечено</t>
   </si>
@@ -286,6 +286,24 @@
   </si>
   <si>
     <t>d239f95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.50, Val IoU: 0.45. </t>
+  </si>
+  <si>
+    <t>a523aff</t>
+  </si>
+  <si>
+    <t>Вместо старой системы аугментации используется улучшенный набор аугментаций из albumentations</t>
+  </si>
+  <si>
+    <t>Изменена система аугментаций</t>
+  </si>
+  <si>
+    <t>fa6507f</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.43, Val IoU: 0.46. Нуждается в доработке</t>
   </si>
 </sst>
 </file>
@@ -736,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,17 +1426,39 @@
       <c r="G25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="13"/>
+      <c r="H25" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>40</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reworked test images directory
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Тесты" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t>Размечено</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Train IoU: 0.43, Val IoU: 0.46. Нуждается в доработке</t>
+  </si>
+  <si>
+    <t>ОБУЧАЮЩИЙ</t>
+  </si>
+  <si>
+    <t>ТЕСТОВЫЙ</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -472,6 +478,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -754,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,9 +1569,14 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -1577,8 +1589,21 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="25"/>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1592,8 +1617,22 @@
       <c r="D2" s="5">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="25"/>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>I2-G2</f>
+        <v>100</v>
+      </c>
+      <c r="I2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1607,8 +1646,22 @@
       <c r="D3" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="25"/>
+      <c r="F3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H6" si="1">I3-G3</f>
+        <v>50</v>
+      </c>
+      <c r="I3" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1622,8 +1675,22 @@
       <c r="D4" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="25"/>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I4" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1637,8 +1704,22 @@
       <c r="D5" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="25"/>
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I5" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1652,19 +1733,53 @@
       <c r="D6" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="25"/>
+      <c r="F6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I6" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <f t="shared" ref="B7:C7" si="1">SUM(B2:B6)</f>
+        <f t="shared" ref="B7:C7" si="2">SUM(B2:B6)</f>
         <v>600</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D7" s="1">
         <f>SUM(D2:D6)</f>
         <v>600</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7:H7" si="3">SUM(G2:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="I7" s="1">
+        <f>SUM(I2:I6)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
loss function changed to IoU + Center Distance
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
   <si>
     <t>Размечено</t>
   </si>
@@ -318,10 +318,22 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Размера батча изменён на 64. </t>
-  </si>
-  <si>
     <t>Train IoU: 0.55, Val IoU: 0.51, Test IoU: 0.50. Дальнейшее изменение размера батча, предположительно, не имеет смысла.</t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на IoU</t>
+  </si>
+  <si>
+    <t>Размера батча изменён на 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.43, Val IoU: 0.43, Test IoU: 0.40. Точность снизилась, но теперь модель более приближена к практической цели своей работы. </t>
+  </si>
+  <si>
+    <t>3c89449</t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на равносильную комбинацию IoU и расстояния между центрами</t>
   </si>
 </sst>
 </file>
@@ -774,7 +786,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,31 +1533,63 @@
         <v>18</v>
       </c>
       <c r="F28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>96</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>19</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="G30" s="8"/>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>40</v>
+      </c>
+      <c r="D30">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H30" s="12"/>
       <c r="I30" s="13"/>
       <c r="J30" s="7"/>

</xml_diff>

<commit_message>
loss function changed to CIoU
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
   <si>
     <t>Размечено</t>
   </si>
@@ -314,26 +314,54 @@
     <t>4527df5</t>
   </si>
   <si>
-    <t xml:space="preserve">4527df5
+    <t>Train IoU: 0.55, Val IoU: 0.51, Test IoU: 0.50. Дальнейшее изменение размера батча, предположительно, не имеет смысла.</t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на IoU</t>
+  </si>
+  <si>
+    <t>Размера батча изменён на 64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.43, Val IoU: 0.43, Test IoU: 0.40. Точность снизилась, но теперь модель более приближена к практической цели своей работы. </t>
+  </si>
+  <si>
+    <t>3c89449</t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на равносильную комбинацию IoU и расстояния между центрами</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.52, Val IoU: 0.56, Test IoU: 0.53. Модель почти достигла предыдущего лучшего результата. Нужно проверять на большем числе эпох и с другими параметрами функции.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d6a497d
 </t>
   </si>
   <si>
-    <t>Train IoU: 0.55, Val IoU: 0.51, Test IoU: 0.50. Дальнейшее изменение размера батча, предположительно, не имеет смысла.</t>
-  </si>
-  <si>
-    <t>Функция потерь заменена на IoU</t>
-  </si>
-  <si>
-    <t>Размера батча изменён на 64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train IoU: 0.43, Val IoU: 0.43, Test IoU: 0.40. Точность снизилась, но теперь модель более приближена к практической цели своей работы. </t>
-  </si>
-  <si>
-    <t>3c89449</t>
-  </si>
-  <si>
-    <t>Функция потерь заменена на равносильную комбинацию IoU и расстояния между центрами</t>
+    <t>Train IoU: 0.60, Val IoU: 0.60, Test IoU: 0.61. Новый лучший результат. Можно работать отсюда.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d6a497d
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.63, Test IoU: 0.61. </t>
+  </si>
+  <si>
+    <t>IoU/Dist = 70/30</t>
+  </si>
+  <si>
+    <t>IoU/Dist = 30/70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.62, Test IoU: 0.64. </t>
+  </si>
+  <si>
+    <t>IoU/Dist = 20/80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.62, Val IoU: 0.61, Test IoU: 0.63. </t>
   </si>
 </sst>
 </file>
@@ -454,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -503,6 +531,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -783,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,7 +900,7 @@
         <v>48</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1533,13 +1563,13 @@
         <v>18</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="7"/>
@@ -1558,20 +1588,20 @@
         <v>19</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H29" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I29" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -1585,60 +1615,251 @@
         <v>20</v>
       </c>
       <c r="F30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="12"/>
-      <c r="I30" s="13"/>
+      <c r="I30" s="15" t="s">
+        <v>101</v>
+      </c>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>80</v>
+      </c>
+      <c r="D31" s="26">
+        <v>20</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="11"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="I31" s="13"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="26">
+        <v>1</v>
+      </c>
+      <c r="C32" s="26">
+        <v>80</v>
+      </c>
+      <c r="D32" s="26">
+        <v>20</v>
+      </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="G38" s="11"/>
+      <c r="F32" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="26">
+        <v>1</v>
+      </c>
+      <c r="C33" s="26">
+        <v>80</v>
+      </c>
+      <c r="D33" s="26">
+        <v>20</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I33" s="27"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="26">
+        <v>1</v>
+      </c>
+      <c r="C34" s="26">
+        <v>100</v>
+      </c>
+      <c r="D34" s="26">
+        <v>20</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="27"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="27"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="27"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="G41" s="8"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="27"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="G42" s="8"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="27"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="27"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="G44" s="8"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="27"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="G45" s="8"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="27"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="G48" s="8"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="27"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="G49" s="8"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="27"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="G50" s="8"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="27"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="G51" s="8"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revert to previous loss function. Modified model to have more depth
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="114">
   <si>
     <t>Размечено</t>
   </si>
@@ -362,6 +362,18 @@
   </si>
   <si>
     <t xml:space="preserve">Train IoU: 0.62, Val IoU: 0.61, Test IoU: 0.63. </t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на более полную - включая IoU, расстояние между центрами, диагональ описывающего прямоугольника и соотношение сторон</t>
+  </si>
+  <si>
+    <t>Лучший результат</t>
+  </si>
+  <si>
+    <t>01213c0</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.56, Val IoU: 0.54, Test IoU: 0.56. Учитывается больше параметров, но модели нужно больше времени на обучение и не факт, что они все важны.</t>
   </si>
 </sst>
 </file>
@@ -387,12 +399,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -482,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -533,6 +551,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -816,7 +847,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,6 +961,9 @@
       <c r="K3" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="L3" s="28" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -1678,28 +1712,29 @@
       <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="A33" s="29">
         <v>32</v>
       </c>
-      <c r="B33" s="26">
-        <v>1</v>
-      </c>
-      <c r="C33" s="26">
+      <c r="B33" s="30">
+        <v>1</v>
+      </c>
+      <c r="C33" s="30">
         <v>80</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="30">
         <v>20</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="E33" s="28"/>
+      <c r="F33" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="G33" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="12" t="s">
+      <c r="G33" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="I33" s="27"/>
+      <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -1725,19 +1760,48 @@
       </c>
       <c r="I34" s="27"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="27"/>
+      <c r="B35" s="26">
+        <v>1</v>
+      </c>
+      <c r="C35" s="26">
+        <v>80</v>
+      </c>
+      <c r="D35" s="26">
+        <v>21</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="G36" s="8"/>
+      <c r="B36" s="26">
+        <v>1</v>
+      </c>
+      <c r="C36" s="26">
+        <v>120</v>
+      </c>
+      <c r="D36" s="26">
+        <v>21</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="12"/>
       <c r="I36" s="27"/>
     </row>

</xml_diff>

<commit_message>
revert some changes to model
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>Размечено</t>
   </si>
@@ -374,6 +374,15 @@
   </si>
   <si>
     <t>Train IoU: 0.56, Val IoU: 0.54, Test IoU: 0.56. Учитывается больше параметров, но модели нужно больше времени на обучение и не факт, что они все важны.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.46, Val IoU: 0.40, Test IoU: 0.36. Сильное переобучение после 80 эпох. Стоит также пока что вернуться к предыдущей функции потерь.</t>
+  </si>
+  <si>
+    <t>Возврат к предыдущей функции потерь. Небольшие изменения в структуре слоёв модели.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.45, Val IoU: 0.52, Test IoU: 0.51. Изменения не дали результата.</t>
   </si>
 </sst>
 </file>
@@ -846,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +1795,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1802,15 +1811,33 @@
       <c r="G36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="I36" s="27"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="12"/>
+      <c r="B37" s="26">
+        <v>1</v>
+      </c>
+      <c r="C37" s="26">
+        <v>80</v>
+      </c>
+      <c r="D37" s="26">
+        <v>22</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>116</v>
+      </c>
       <c r="I37" s="27"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
functions split into separate modules
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
   <si>
     <t>Размечено</t>
   </si>
@@ -342,59 +342,62 @@
     <t>Train IoU: 0.60, Val IoU: 0.60, Test IoU: 0.61. Новый лучший результат. Можно работать отсюда.</t>
   </si>
   <si>
-    <t xml:space="preserve">d6a497d
+    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.63, Test IoU: 0.61. </t>
+  </si>
+  <si>
+    <t>IoU/Dist = 70/30</t>
+  </si>
+  <si>
+    <t>IoU/Dist = 30/70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.62, Test IoU: 0.64. </t>
+  </si>
+  <si>
+    <t>IoU/Dist = 20/80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.62, Val IoU: 0.61, Test IoU: 0.63. </t>
+  </si>
+  <si>
+    <t>Функция потерь заменена на более полную - включая IoU, расстояние между центрами, диагональ описывающего прямоугольника и соотношение сторон</t>
+  </si>
+  <si>
+    <t>Лучший результат</t>
+  </si>
+  <si>
+    <t>01213c0</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.56, Val IoU: 0.54, Test IoU: 0.56. Учитывается больше параметров, но модели нужно больше времени на обучение и не факт, что они все важны.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.46, Val IoU: 0.40, Test IoU: 0.36. Сильное переобучение после 80 эпох. Стоит также пока что вернуться к предыдущей функции потерь.</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.45, Val IoU: 0.52, Test IoU: 0.51. Изменения не дали результата.</t>
+  </si>
+  <si>
+    <t>Откат некоторых изменений модели предыдущей версии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train IoU: 0.61, Val IoU: 0.62, Test IoU: 0.62. Модель близка к точке переобучения, но нужно проверить на чуть большем числе эпох. </t>
+  </si>
+  <si>
+    <t>6fb9b16</t>
+  </si>
+  <si>
+    <t>419a033</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.65, Val IoU: 0.64, Test IoU: 0.66.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0879013
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.63, Test IoU: 0.61. </t>
-  </si>
-  <si>
-    <t>IoU/Dist = 70/30</t>
-  </si>
-  <si>
-    <t>IoU/Dist = 30/70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train IoU: 0.59, Val IoU: 0.62, Test IoU: 0.64. </t>
-  </si>
-  <si>
-    <t>IoU/Dist = 20/80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train IoU: 0.62, Val IoU: 0.61, Test IoU: 0.63. </t>
-  </si>
-  <si>
-    <t>Функция потерь заменена на более полную - включая IoU, расстояние между центрами, диагональ описывающего прямоугольника и соотношение сторон</t>
-  </si>
-  <si>
-    <t>Лучший результат</t>
-  </si>
-  <si>
-    <t>01213c0</t>
-  </si>
-  <si>
-    <t>Train IoU: 0.56, Val IoU: 0.54, Test IoU: 0.56. Учитывается больше параметров, но модели нужно больше времени на обучение и не факт, что они все важны.</t>
-  </si>
-  <si>
-    <t>Train IoU: 0.46, Val IoU: 0.40, Test IoU: 0.36. Сильное переобучение после 80 эпох. Стоит также пока что вернуться к предыдущей функции потерь.</t>
-  </si>
-  <si>
-    <t>Возврат к предыдущей функции потерь. Небольшие изменения в структуре слоёв модели.</t>
-  </si>
-  <si>
-    <t>Train IoU: 0.45, Val IoU: 0.52, Test IoU: 0.51. Изменения не дали результата.</t>
-  </si>
-  <si>
-    <t>Откат некоторых изменений модели предыдущей версии</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train IoU: 0.61, Val IoU: 0.62, Test IoU: 0.62. Модель близка к точке переобучения, но нужно проверить на чуть большем числе эпох. </t>
-  </si>
-  <si>
-    <t>6fb9b16</t>
-  </si>
-  <si>
-    <t>419a033</t>
+    <t>Возврат к предыдущей функции потерь (пропорция 30/70). Небольшие изменения в структуре слоёв модели.</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -573,6 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -585,6 +589,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -867,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,7 +967,7 @@
         <v>48</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -983,7 +998,7 @@
         <v>14</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1722,40 +1737,40 @@
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="36">
+        <v>32</v>
+      </c>
+      <c r="B33" s="26">
+        <v>1</v>
+      </c>
+      <c r="C33" s="26">
+        <v>80</v>
+      </c>
+      <c r="D33" s="26">
+        <v>20</v>
+      </c>
+      <c r="E33" s="29"/>
+      <c r="F33" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="I32" s="27"/>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
-        <v>32</v>
-      </c>
-      <c r="B33" s="30">
-        <v>1</v>
-      </c>
-      <c r="C33" s="30">
-        <v>80</v>
-      </c>
-      <c r="D33" s="30">
-        <v>20</v>
-      </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="31" t="s">
+      <c r="G33" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="G33" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="I33" s="34"/>
+      <c r="I33" s="40"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
@@ -1771,13 +1786,13 @@
         <v>20</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>109</v>
       </c>
       <c r="I34" s="27"/>
     </row>
@@ -1795,16 +1810,16 @@
         <v>21</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I35" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1824,11 +1839,11 @@
         <v>29</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I36" s="27"/>
     </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1842,16 +1857,16 @@
         <v>22</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1868,36 +1883,40 @@
         <v>23</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I38" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="I38" s="27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="30">
         <v>38</v>
       </c>
-      <c r="B39" s="26">
-        <v>1</v>
-      </c>
-      <c r="C39" s="26">
+      <c r="B39" s="31">
+        <v>1</v>
+      </c>
+      <c r="C39" s="31">
         <v>100</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="31">
         <v>23</v>
       </c>
-      <c r="G39" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="27"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="32"/>
+      <c r="G39" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="35"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="6">

</xml_diff>

<commit_message>
image resize changed from 320x320 to 400x400
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="125">
   <si>
     <t>Размечено</t>
   </si>
@@ -393,11 +393,20 @@
     <t>Train IoU: 0.65, Val IoU: 0.64, Test IoU: 0.66.</t>
   </si>
   <si>
-    <t xml:space="preserve">0879013
+    <t>Возврат к предыдущей функции потерь (пропорция 30/70). Небольшие изменения в структуре слоёв модели.</t>
+  </si>
+  <si>
+    <t>Замена базовой модели с resnet18 на resnet34, добавлен 4 слой</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.67, Val IoU: 0.70, Test IoU: 0.71.</t>
+  </si>
+  <si>
+    <t>bd81fa3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bd81fa3
 </t>
-  </si>
-  <si>
-    <t>Возврат к предыдущей функции потерь (пропорция 30/70). Небольшие изменения в структуре слоёв модели.</t>
   </si>
 </sst>
 </file>
@@ -882,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +976,7 @@
         <v>48</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1857,7 +1866,7 @@
         <v>22</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>29</v>
@@ -1896,35 +1905,54 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="30">
+      <c r="A39" s="36">
         <v>38</v>
       </c>
-      <c r="B39" s="31">
-        <v>1</v>
-      </c>
-      <c r="C39" s="31">
+      <c r="B39" s="26">
+        <v>1</v>
+      </c>
+      <c r="C39" s="26">
         <v>100</v>
       </c>
-      <c r="D39" s="31">
+      <c r="D39" s="26">
         <v>23</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="H39" s="34" t="s">
+      <c r="E39" s="29"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="I39" s="35"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="I39" s="40"/>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="30">
         <v>39</v>
       </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="27"/>
+      <c r="B40" s="31">
+        <v>1</v>
+      </c>
+      <c r="C40" s="31">
+        <v>100</v>
+      </c>
+      <c r="D40" s="31">
+        <v>24</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I40" s="35" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="6">

</xml_diff>

<commit_message>
revert to version 24
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
   <si>
     <t>Размечено</t>
   </si>
@@ -413,6 +413,18 @@
   </si>
   <si>
     <t>Train IoU: 0.61, Val IoU: 0.65, Test IoU: 0.67.</t>
+  </si>
+  <si>
+    <t>Adaptive pool увеличен с (4,4) до (7,7)</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.64, Val IoU: 0.64, Test IoU: 0.64.</t>
+  </si>
+  <si>
+    <t>Adaptive pool уменьшен с (7,7) до (5,5)</t>
+  </si>
+  <si>
+    <t>Train IoU: 0.66, Val IoU: 0.67, Test IoU: 0.68.</t>
   </si>
 </sst>
 </file>
@@ -898,7 +910,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,20 +1993,52 @@
       </c>
       <c r="I41" s="27"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="G42" s="8"/>
-      <c r="H42" s="12"/>
+      <c r="B42" s="26">
+        <v>1</v>
+      </c>
+      <c r="C42" s="26">
+        <v>100</v>
+      </c>
+      <c r="D42" s="26">
+        <v>25</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>128</v>
+      </c>
       <c r="I42" s="27"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="12"/>
+      <c r="B43" s="26">
+        <v>1</v>
+      </c>
+      <c r="C43" s="26">
+        <v>100</v>
+      </c>
+      <c r="D43" s="26">
+        <v>26</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added classification model training on full images. Reorganized files to run pipeline from one file.
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
   <si>
     <t>Размечено</t>
   </si>
@@ -425,6 +425,22 @@
   </si>
   <si>
     <t>Train IoU: 0.66, Val IoU: 0.67, Test IoU: 0.68.</t>
+  </si>
+  <si>
+    <t>Базовая версия модели классификатора</t>
+  </si>
+  <si>
+    <t>86b705a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22e3876
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точность: Train: 83.5%, Val: 80.5%, Test: 63.3%. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точность: Train: 74.2%, Val: 63.7%, Test: 64%. </t>
   </si>
 </sst>
 </file>
@@ -551,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -627,6 +643,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -910,7 +929,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,7 +2034,9 @@
       <c r="H42" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="I42" s="27"/>
+      <c r="I42" s="41" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
@@ -2041,21 +2062,61 @@
       </c>
       <c r="I43" s="27"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43</v>
       </c>
-      <c r="G44" s="8"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="27"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="B44" s="26">
+        <v>2</v>
+      </c>
+      <c r="C44" s="26">
+        <v>100</v>
+      </c>
+      <c r="D44" s="26">
+        <v>24</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="30">
         <v>44</v>
       </c>
-      <c r="G45" s="8"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="27"/>
+      <c r="B45" s="31">
+        <v>2</v>
+      </c>
+      <c r="C45" s="31">
+        <v>100</v>
+      </c>
+      <c r="D45" s="31">
+        <v>24</v>
+      </c>
+      <c r="E45" s="31">
+        <v>1</v>
+      </c>
+      <c r="F45" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="I45" s="35"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6">

</xml_diff>

<commit_message>
added base model efficientnet b0 for classification
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
   <si>
     <t>Размечено</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Модель</t>
-  </si>
-  <si>
-    <t>Эпох</t>
   </si>
   <si>
     <t>Номер теста</t>
@@ -363,9 +360,6 @@
     <t>Функция потерь заменена на более полную - включая IoU, расстояние между центрами, диагональ описывающего прямоугольника и соотношение сторон</t>
   </si>
   <si>
-    <t>Лучший результат</t>
-  </si>
-  <si>
     <t>01213c0</t>
   </si>
   <si>
@@ -403,10 +397,6 @@
   </si>
   <si>
     <t>bd81fa3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bd81fa3
-</t>
   </si>
   <si>
     <t>параметры теста 4, но resize в 400x400</t>
@@ -441,6 +431,40 @@
   </si>
   <si>
     <t xml:space="preserve">Точность: Train: 74.2%, Val: 63.7%, Test: 64%. </t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 87.6%</t>
+  </si>
+  <si>
+    <t>Порог уверенности для использования данных с обрезанным первой моделью кодом увеличен до 1.</t>
+  </si>
+  <si>
+    <t>Лучший результат (1 модель)</t>
+  </si>
+  <si>
+    <t>Лучший результат (2 модель)</t>
+  </si>
+  <si>
+    <t>b9c54e7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b9c54e7
+</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 90.6%</t>
+  </si>
+  <si>
+    <t>100/50</t>
+  </si>
+  <si>
+    <t>120/100</t>
+  </si>
+  <si>
+    <t>100/100</t>
+  </si>
+  <si>
+    <t>Эпох(1 модель/2 модель)</t>
   </si>
 </sst>
 </file>
@@ -466,7 +490,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +500,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -646,6 +682,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -929,12 +978,13 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -948,38 +998,38 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>19</v>
-      </c>
       <c r="I1" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="23"/>
       <c r="K1" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -996,24 +1046,24 @@
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="7"/>
       <c r="K2" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1030,21 +1080,21 @@
         <v>2</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="7"/>
       <c r="K3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -1061,18 +1111,21 @@
         <v>3</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="7"/>
+      <c r="L4" s="42" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -1088,16 +1141,16 @@
         <v>4</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>35</v>
       </c>
       <c r="J5" s="7"/>
     </row>
@@ -1115,10 +1168,10 @@
         <v>4</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="7"/>
@@ -1137,10 +1190,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="7"/>
@@ -1159,10 +1212,10 @@
         <v>4</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="7"/>
@@ -1181,16 +1234,16 @@
         <v>5</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="J9" s="7"/>
     </row>
@@ -1208,16 +1261,16 @@
         <v>6</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="13" t="s">
         <v>40</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>41</v>
       </c>
       <c r="J10" s="7"/>
     </row>
@@ -1235,10 +1288,10 @@
         <v>6</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="7"/>
@@ -1257,16 +1310,16 @@
         <v>7</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="J12" s="7"/>
       <c r="K12" s="16"/>
@@ -1285,16 +1338,16 @@
         <v>8</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="I13" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>51</v>
       </c>
       <c r="J13" s="7"/>
     </row>
@@ -1312,10 +1365,10 @@
         <v>8</v>
       </c>
       <c r="G14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>52</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>53</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="7"/>
@@ -1334,16 +1387,16 @@
         <v>9</v>
       </c>
       <c r="F15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="I15" s="15" t="s">
         <v>56</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="J15" s="7"/>
     </row>
@@ -1361,16 +1414,16 @@
         <v>10</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="J16" s="7"/>
     </row>
@@ -1388,16 +1441,16 @@
         <v>11</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="J17" s="7"/>
     </row>
@@ -1415,16 +1468,16 @@
         <v>12</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>65</v>
       </c>
       <c r="J18" s="7"/>
     </row>
@@ -1442,16 +1495,16 @@
         <v>13</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="7"/>
     </row>
@@ -1469,13 +1522,13 @@
         <v>13</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="7"/>
@@ -1494,13 +1547,13 @@
         <v>13</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="I21" s="13"/>
       <c r="J21" s="7"/>
@@ -1519,16 +1572,16 @@
         <v>14</v>
       </c>
       <c r="F22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>75</v>
-      </c>
       <c r="I22" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J22" s="7"/>
     </row>
@@ -1546,13 +1599,13 @@
         <v>14</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I23" s="13"/>
       <c r="J23" s="7"/>
@@ -1571,16 +1624,16 @@
         <v>15</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>80</v>
-      </c>
       <c r="I24" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J24" s="7"/>
     </row>
@@ -1598,16 +1651,16 @@
         <v>16</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="J25" s="7"/>
     </row>
@@ -1625,16 +1678,16 @@
         <v>17</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I26" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="J26" s="7"/>
     </row>
@@ -1652,16 +1705,16 @@
         <v>18</v>
       </c>
       <c r="F27" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="12" t="s">
+      <c r="I27" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="I27" s="13" t="s">
-        <v>93</v>
       </c>
       <c r="J27" s="7"/>
     </row>
@@ -1679,13 +1732,13 @@
         <v>18</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="7"/>
@@ -1704,16 +1757,16 @@
         <v>19</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="J29" s="7"/>
     </row>
@@ -1731,16 +1784,16 @@
         <v>20</v>
       </c>
       <c r="F30" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="12" t="s">
+      <c r="I30" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="J30" s="7"/>
     </row>
@@ -1760,10 +1813,10 @@
       <c r="E31" s="7"/>
       <c r="F31" s="11"/>
       <c r="G31" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="7"/>
@@ -1783,13 +1836,13 @@
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I32" s="27"/>
     </row>
@@ -1808,13 +1861,13 @@
       </c>
       <c r="E33" s="29"/>
       <c r="F33" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="39" t="s">
         <v>105</v>
-      </c>
-      <c r="G33" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="39" t="s">
-        <v>106</v>
       </c>
       <c r="I33" s="40"/>
     </row>
@@ -1832,13 +1885,13 @@
         <v>20</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="I34" s="27"/>
     </row>
@@ -1856,16 +1909,16 @@
         <v>21</v>
       </c>
       <c r="F35" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I35" s="27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1882,10 +1935,10 @@
         <v>21</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I36" s="27"/>
     </row>
@@ -1903,16 +1956,16 @@
         <v>22</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I37" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1929,16 +1982,16 @@
         <v>23</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H38" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I38" s="27" t="s">
         <v>116</v>
-      </c>
-      <c r="I38" s="27" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1957,10 +2010,10 @@
       <c r="E39" s="29"/>
       <c r="F39" s="37"/>
       <c r="G39" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H39" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I39" s="40"/>
     </row>
@@ -1979,16 +2032,16 @@
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="I40" s="35" t="s">
         <v>121</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="H40" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="I40" s="35" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2005,10 +2058,10 @@
         <v>24</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I41" s="27"/>
     </row>
@@ -2026,16 +2079,16 @@
         <v>25</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I42" s="41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2052,13 +2105,13 @@
         <v>26</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I43" s="27"/>
     </row>
@@ -2069,8 +2122,8 @@
       <c r="B44" s="26">
         <v>2</v>
       </c>
-      <c r="C44" s="26">
-        <v>100</v>
+      <c r="C44" s="26" t="s">
+        <v>142</v>
       </c>
       <c r="D44" s="26">
         <v>24</v>
@@ -2079,60 +2132,96 @@
         <v>1</v>
       </c>
       <c r="F44" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="12" t="s">
+      <c r="I44" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="36">
+        <v>44</v>
+      </c>
+      <c r="B45" s="26">
+        <v>2</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="26">
+        <v>24</v>
+      </c>
+      <c r="E45" s="26">
+        <v>1</v>
+      </c>
+      <c r="F45" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="G45" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="I45" s="40"/>
+    </row>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="36">
+        <v>45</v>
+      </c>
+      <c r="B46" s="26">
+        <v>2</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="26">
+        <v>24</v>
+      </c>
+      <c r="E46" s="26">
+        <v>2</v>
+      </c>
+      <c r="F46" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="I44" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="30">
-        <v>44</v>
-      </c>
-      <c r="B45" s="31">
+      <c r="G46" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="I46" s="40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="43">
+        <v>46</v>
+      </c>
+      <c r="B47" s="44">
         <v>2</v>
       </c>
-      <c r="C45" s="31">
-        <v>100</v>
-      </c>
-      <c r="D45" s="31">
+      <c r="C47" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="44">
         <v>24</v>
       </c>
-      <c r="E45" s="31">
-        <v>1</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="G45" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="H45" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I45" s="35"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="6">
-        <v>45</v>
-      </c>
-      <c r="G46" s="8"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="27"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="6">
-        <v>46</v>
-      </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="27"/>
+      <c r="E47" s="44">
+        <v>2</v>
+      </c>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="I47" s="48"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
@@ -2392,10 +2481,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
         <v>89</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing 20 epochs on classification, full model 2 results
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="147">
   <si>
     <t>Размечено</t>
   </si>
@@ -448,23 +448,32 @@
     <t>b9c54e7</t>
   </si>
   <si>
-    <t xml:space="preserve">b9c54e7
+    <t>Точность на тестовых данных: 90.6%</t>
+  </si>
+  <si>
+    <t>100/50</t>
+  </si>
+  <si>
+    <t>120/100</t>
+  </si>
+  <si>
+    <t>100/100</t>
+  </si>
+  <si>
+    <t>Эпох(1 модель/2 модель)</t>
+  </si>
+  <si>
+    <t>Базовая классификационная модель заменена на EfficientNet B0</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 98.3%</t>
+  </si>
+  <si>
+    <t>f643650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f643650
 </t>
-  </si>
-  <si>
-    <t>Точность на тестовых данных: 90.6%</t>
-  </si>
-  <si>
-    <t>100/50</t>
-  </si>
-  <si>
-    <t>120/100</t>
-  </si>
-  <si>
-    <t>100/100</t>
-  </si>
-  <si>
-    <t>Эпох(1 модель/2 модель)</t>
   </si>
 </sst>
 </file>
@@ -977,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1013,7 @@
         <v>9</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>14</v>
@@ -1063,7 +1072,7 @@
         <v>47</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2123,7 +2132,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D44" s="26">
         <v>24</v>
@@ -2152,7 +2161,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D45" s="26">
         <v>24</v>
@@ -2179,7 +2188,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="26">
         <v>24</v>
@@ -2201,35 +2210,58 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="43">
+      <c r="A47" s="36">
         <v>46</v>
       </c>
-      <c r="B47" s="44">
+      <c r="B47" s="26">
         <v>2</v>
       </c>
-      <c r="C47" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="44">
+      <c r="C47" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="26">
         <v>24</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="26">
         <v>2</v>
       </c>
-      <c r="F47" s="45"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="47" t="s">
+      <c r="F47" s="37"/>
+      <c r="G47" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="I47" s="40"/>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="43">
+        <v>47</v>
+      </c>
+      <c r="B48" s="44">
+        <v>2</v>
+      </c>
+      <c r="C48" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="I47" s="48"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
-        <v>47</v>
-      </c>
-      <c r="G48" s="8"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="27"/>
+      <c r="D48" s="44">
+        <v>24</v>
+      </c>
+      <c r="E48" s="44">
+        <v>3</v>
+      </c>
+      <c r="F48" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="I48" s="48" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="6">

</xml_diff>

<commit_message>
object detection model update, testing with threshold 0
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -472,20 +472,21 @@
     <t>f643650</t>
   </si>
   <si>
-    <t xml:space="preserve">f643650
+    <t>100/20</t>
+  </si>
+  <si>
+    <t>Порог уверенности повышен до 1.1 (все результаты берутся из 2 модели)</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8935088
 </t>
   </si>
   <si>
-    <t>100/20</t>
-  </si>
-  <si>
-    <t>Порог уверенности повышен до 1.1 (все результаты берутся из 2 модели)</t>
-  </si>
-  <si>
-    <t>Точность на тестовых данных: 100%</t>
-  </si>
-  <si>
-    <t>f602d46</t>
+    <t xml:space="preserve">8935088
+</t>
   </si>
 </sst>
 </file>
@@ -715,7 +716,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -998,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1087,7 @@
         <v>47</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -2283,7 +2286,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D49" s="44">
         <v>24</v>
@@ -2292,16 +2295,16 @@
         <v>3</v>
       </c>
       <c r="F49" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="G49" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H49" s="47" t="s">
+      <c r="I49" s="48" t="s">
         <v>149</v>
-      </c>
-      <c r="I49" s="48" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
testing efficientnet on bbox model
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="163">
   <si>
     <t>Размечено</t>
   </si>
@@ -487,6 +487,42 @@
   <si>
     <t xml:space="preserve">8935088
 </t>
+  </si>
+  <si>
+    <t>80/20</t>
+  </si>
+  <si>
+    <t>Небольшие изменения в структуре первой модели, порог для теста изменён до 0 (все результаты берутся из 1 модели)</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 91.3%</t>
+  </si>
+  <si>
+    <t>325f8c6</t>
+  </si>
+  <si>
+    <t>Порог изменён на 0.6</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 93.7%</t>
+  </si>
+  <si>
+    <t>Порог изменён на 0.8</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 95.3%</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 97.7%</t>
+  </si>
+  <si>
+    <t>Порог изменён на 0.95</t>
+  </si>
+  <si>
+    <t>Порог изменён на 1</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 99%</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,21 +2343,318 @@
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="27"/>
+      <c r="B50" s="26">
+        <v>2</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="26">
+        <v>25</v>
+      </c>
+      <c r="E50" s="26">
+        <v>3</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>50</v>
       </c>
-      <c r="G51" s="8"/>
-      <c r="H51" s="12"/>
+      <c r="B51" s="26">
+        <v>2</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="26">
+        <v>25</v>
+      </c>
+      <c r="E51" s="26">
+        <v>3</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>156</v>
+      </c>
       <c r="I51" s="27"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="26">
+        <v>2</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="26">
+        <v>25</v>
+      </c>
+      <c r="E52" s="26">
+        <v>3</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I52" s="27"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="26">
+        <v>2</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D53" s="26">
+        <v>25</v>
+      </c>
+      <c r="E53" s="26">
+        <v>3</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I53" s="27"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="26">
+        <v>2</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" s="26">
+        <v>25</v>
+      </c>
+      <c r="E54" s="26">
+        <v>3</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I54" s="27"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="27"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="27"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="27"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="27"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="G60" s="8"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="27"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="G61" s="8"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="27"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="G62" s="8"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="27"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="G63" s="8"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="27"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="27"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="27"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="G66" s="8"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="27"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="G67" s="8"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="27"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>67</v>
+      </c>
+      <c r="G68" s="8"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="27"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="27"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>69</v>
+      </c>
+      <c r="G70" s="8"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="27"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>70</v>
+      </c>
+      <c r="G71" s="8"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="27"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="G72" s="8"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="27"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="G73" s="8"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="27"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>73</v>
+      </c>
+      <c r="G74" s="8"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="27"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="G75" s="8"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="27"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>75</v>
+      </c>
+      <c r="G76" s="8"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revert to version 24-3
</commit_message>
<xml_diff>
--- a/media/meta.xlsx
+++ b/media/meta.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="167">
   <si>
     <t>Размечено</t>
   </si>
@@ -523,6 +523,18 @@
   </si>
   <si>
     <t>Точность на тестовых данных: 99%</t>
+  </si>
+  <si>
+    <t>Базовая модель первой модели заменена на EfficientNet B0.</t>
+  </si>
+  <si>
+    <t>296ea60</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 98%</t>
+  </si>
+  <si>
+    <t>Точность на тестовых данных: 99.67%</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,28 +2492,87 @@
       </c>
       <c r="I54" s="27"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>54</v>
       </c>
-      <c r="G55" s="8"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="27"/>
+      <c r="B55" s="26">
+        <v>2</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" s="26">
+        <v>26</v>
+      </c>
+      <c r="E55" s="26">
+        <v>3</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I55" s="27" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>55</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="12"/>
+      <c r="B56" s="26">
+        <v>2</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="26">
+        <v>26</v>
+      </c>
+      <c r="E56" s="26">
+        <v>3</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="I56" s="27"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>56</v>
       </c>
-      <c r="G57" s="8"/>
-      <c r="H57" s="12"/>
+      <c r="B57" s="26">
+        <v>2</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="26">
+        <v>26</v>
+      </c>
+      <c r="E57" s="26">
+        <v>3</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>166</v>
+      </c>
       <c r="I57" s="27"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>